<commit_message>
more bugfixing of all cars
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -8,13 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Počty vozidel" sheetId="1" r:id="rId1"/>
+    <sheet name="Počty vozidel_04.50_09.00" sheetId="2" r:id="rId2"/>
+    <sheet name="Počty vozidel_03.00_10.00" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="25">
   <si>
     <t>Základní výstupní tabulky (počty všech vozidel)</t>
   </si>
@@ -677,7 +679,7 @@
         <v>3</v>
       </c>
       <c r="T5">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -737,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -799,7 +801,7 @@
         <v>27</v>
       </c>
       <c r="T7">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -859,7 +861,7 @@
         <v>24</v>
       </c>
       <c r="T8">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -921,7 +923,7 @@
         <v>7</v>
       </c>
       <c r="T9">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -981,7 +983,7 @@
         <v>15</v>
       </c>
       <c r="T10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1043,7 +1045,7 @@
         <v>1</v>
       </c>
       <c r="T11">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1103,7 +1105,7 @@
         <v>3</v>
       </c>
       <c r="T12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1165,7 +1167,7 @@
         <v>8</v>
       </c>
       <c r="T13">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1225,7 +1227,7 @@
         <v>8</v>
       </c>
       <c r="T14">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1287,7 +1289,7 @@
         <v>0</v>
       </c>
       <c r="T15">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1347,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="T16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -1409,7 +1411,7 @@
         <v>2</v>
       </c>
       <c r="T17">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -1469,7 +1471,7 @@
         <v>0</v>
       </c>
       <c r="T18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -1531,7 +1533,7 @@
         <v>13</v>
       </c>
       <c r="T19">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -1591,7 +1593,7 @@
         <v>21</v>
       </c>
       <c r="T20">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -1653,7 +1655,7 @@
         <v>37</v>
       </c>
       <c r="T21">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -1713,7 +1715,7 @@
         <v>49</v>
       </c>
       <c r="T22">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -1770,31 +1772,31 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26">
-        <v>1561</v>
+        <v>1107</v>
       </c>
       <c r="D26">
-        <v>6089</v>
+        <v>2060</v>
       </c>
       <c r="E26">
-        <v>3843</v>
+        <v>468</v>
       </c>
       <c r="F26">
-        <v>3005</v>
+        <v>458</v>
       </c>
       <c r="G26">
-        <v>7840</v>
+        <v>975</v>
       </c>
       <c r="H26">
-        <v>3291</v>
+        <v>873</v>
       </c>
       <c r="I26">
-        <v>4284</v>
+        <v>1071</v>
       </c>
       <c r="J26">
-        <v>2985</v>
+        <v>1098</v>
       </c>
       <c r="K26">
-        <v>2039</v>
+        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:20">
@@ -1851,31 +1853,2919 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30">
-        <v>1820</v>
+        <v>1048</v>
       </c>
       <c r="D30">
-        <v>5823</v>
+        <v>1567</v>
       </c>
       <c r="E30">
-        <v>3499</v>
+        <v>674</v>
       </c>
       <c r="F30">
-        <v>3225</v>
+        <v>455</v>
       </c>
       <c r="G30">
-        <v>7133</v>
+        <v>789</v>
       </c>
       <c r="H30">
-        <v>3992</v>
+        <v>1798</v>
       </c>
       <c r="I30">
-        <v>3697</v>
+        <v>1020</v>
       </c>
       <c r="J30">
-        <v>3173</v>
+        <v>962</v>
       </c>
       <c r="K30">
-        <v>1686</v>
+        <v>705</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A28:K28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A30:B30"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C26:K26">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30:K30">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:T22">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="23" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2">
+        <v>4</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2">
+        <v>5</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2">
+        <v>6</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2">
+        <v>7</v>
+      </c>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2">
+        <v>8</v>
+      </c>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2">
+        <v>9</v>
+      </c>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>4</v>
+      </c>
+      <c r="G4" s="3">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3">
+        <v>7</v>
+      </c>
+      <c r="J4" s="3">
+        <v>8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>9</v>
+      </c>
+      <c r="L4" s="3">
+        <v>10</v>
+      </c>
+      <c r="M4" s="3">
+        <v>11</v>
+      </c>
+      <c r="N4" s="3">
+        <v>12</v>
+      </c>
+      <c r="O4" s="3">
+        <v>13</v>
+      </c>
+      <c r="P4" s="3">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>15</v>
+      </c>
+      <c r="R4" s="3">
+        <v>16</v>
+      </c>
+      <c r="S4" s="3">
+        <v>17</v>
+      </c>
+      <c r="T4" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>24</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>9</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="2">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9">
+        <v>70</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>64</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>37</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>16</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>19</v>
+      </c>
+      <c r="S9">
+        <v>2</v>
+      </c>
+      <c r="T9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>63</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>2</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="2">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>51</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>66</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <v>49</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>7</v>
+      </c>
+      <c r="Q11">
+        <v>3</v>
+      </c>
+      <c r="R11">
+        <v>46</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>31</v>
+      </c>
+      <c r="J12">
+        <v>7</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="2">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>72</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>55</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>68</v>
+      </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <v>172</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>11</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>46</v>
+      </c>
+      <c r="S13">
+        <v>3</v>
+      </c>
+      <c r="T13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>7</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>30</v>
+      </c>
+      <c r="L14">
+        <v>8</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>11</v>
+      </c>
+      <c r="P14">
+        <v>77</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="R14">
+        <v>16</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="2">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="2">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>31</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>52</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>32</v>
+      </c>
+      <c r="K17">
+        <v>352</v>
+      </c>
+      <c r="L17">
+        <v>31</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>10</v>
+      </c>
+      <c r="P17">
+        <v>41</v>
+      </c>
+      <c r="Q17">
+        <v>4</v>
+      </c>
+      <c r="R17">
+        <v>38</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>16</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>31</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="2">
+        <v>8</v>
+      </c>
+      <c r="B19" s="3">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>28</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>107</v>
+      </c>
+      <c r="K19">
+        <v>26</v>
+      </c>
+      <c r="L19">
+        <v>32</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>24</v>
+      </c>
+      <c r="Q19">
+        <v>12</v>
+      </c>
+      <c r="R19">
+        <v>48</v>
+      </c>
+      <c r="S19">
+        <v>5</v>
+      </c>
+      <c r="T19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>36</v>
+      </c>
+      <c r="R20">
+        <v>7</v>
+      </c>
+      <c r="S20">
+        <v>6</v>
+      </c>
+      <c r="T20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="2">
+        <v>9</v>
+      </c>
+      <c r="B21" s="3">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>28</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>32</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>12</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>12</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>3</v>
+      </c>
+      <c r="R21">
+        <v>11</v>
+      </c>
+      <c r="S21">
+        <v>7</v>
+      </c>
+      <c r="T21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>3</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>12</v>
+      </c>
+      <c r="T22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>291</v>
+      </c>
+      <c r="E26">
+        <v>331</v>
+      </c>
+      <c r="F26">
+        <v>367</v>
+      </c>
+      <c r="G26">
+        <v>1213</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>1340</v>
+      </c>
+      <c r="J26">
+        <v>841</v>
+      </c>
+      <c r="K26">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>149</v>
+      </c>
+      <c r="E30">
+        <v>1016</v>
+      </c>
+      <c r="F30">
+        <v>492</v>
+      </c>
+      <c r="G30">
+        <v>801</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>379</v>
+      </c>
+      <c r="J30">
+        <v>541</v>
+      </c>
+      <c r="K30">
+        <v>311</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A28:K28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A30:B30"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C26:K26">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30:K30">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:T22">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="23" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2">
+        <v>4</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2">
+        <v>5</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2">
+        <v>6</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2">
+        <v>7</v>
+      </c>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2">
+        <v>8</v>
+      </c>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2">
+        <v>9</v>
+      </c>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>4</v>
+      </c>
+      <c r="G4" s="3">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3">
+        <v>7</v>
+      </c>
+      <c r="J4" s="3">
+        <v>8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>9</v>
+      </c>
+      <c r="L4" s="3">
+        <v>10</v>
+      </c>
+      <c r="M4" s="3">
+        <v>11</v>
+      </c>
+      <c r="N4" s="3">
+        <v>12</v>
+      </c>
+      <c r="O4" s="3">
+        <v>13</v>
+      </c>
+      <c r="P4" s="3">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>15</v>
+      </c>
+      <c r="R4" s="3">
+        <v>16</v>
+      </c>
+      <c r="S4" s="3">
+        <v>17</v>
+      </c>
+      <c r="T4" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>69</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>19</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>72</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>31</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="R7">
+        <v>6</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="2">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>26</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>102</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>82</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>47</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>3</v>
+      </c>
+      <c r="P9">
+        <v>20</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>24</v>
+      </c>
+      <c r="S9">
+        <v>2</v>
+      </c>
+      <c r="T9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>83</v>
+      </c>
+      <c r="H10">
+        <v>16</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>2</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="2">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>66</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <v>101</v>
+      </c>
+      <c r="K11">
+        <v>8</v>
+      </c>
+      <c r="L11">
+        <v>68</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>12</v>
+      </c>
+      <c r="Q11">
+        <v>7</v>
+      </c>
+      <c r="R11">
+        <v>78</v>
+      </c>
+      <c r="S11">
+        <v>4</v>
+      </c>
+      <c r="T11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>43</v>
+      </c>
+      <c r="J12">
+        <v>15</v>
+      </c>
+      <c r="K12">
+        <v>5</v>
+      </c>
+      <c r="L12">
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="2">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>14</v>
+      </c>
+      <c r="F13">
+        <v>186</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>70</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>103</v>
+      </c>
+      <c r="K13">
+        <v>7</v>
+      </c>
+      <c r="L13">
+        <v>261</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>3</v>
+      </c>
+      <c r="P13">
+        <v>20</v>
+      </c>
+      <c r="Q13">
+        <v>9</v>
+      </c>
+      <c r="R13">
+        <v>70</v>
+      </c>
+      <c r="S13">
+        <v>4</v>
+      </c>
+      <c r="T13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>8</v>
+      </c>
+      <c r="K14">
+        <v>35</v>
+      </c>
+      <c r="L14">
+        <v>14</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>14</v>
+      </c>
+      <c r="P14">
+        <v>89</v>
+      </c>
+      <c r="Q14">
+        <v>4</v>
+      </c>
+      <c r="R14">
+        <v>16</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="2">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="2">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>70</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>60</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>42</v>
+      </c>
+      <c r="K17">
+        <v>382</v>
+      </c>
+      <c r="L17">
+        <v>42</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>15</v>
+      </c>
+      <c r="P17">
+        <v>97</v>
+      </c>
+      <c r="Q17">
+        <v>6</v>
+      </c>
+      <c r="R17">
+        <v>42</v>
+      </c>
+      <c r="S17">
+        <v>2</v>
+      </c>
+      <c r="T17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>26</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>54</v>
+      </c>
+      <c r="P18">
+        <v>3</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <v>3</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="2">
+        <v>8</v>
+      </c>
+      <c r="B19" s="3">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>32</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <v>121</v>
+      </c>
+      <c r="K19">
+        <v>35</v>
+      </c>
+      <c r="L19">
+        <v>39</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+      <c r="P19">
+        <v>26</v>
+      </c>
+      <c r="Q19">
+        <v>13</v>
+      </c>
+      <c r="R19">
+        <v>92</v>
+      </c>
+      <c r="S19">
+        <v>6</v>
+      </c>
+      <c r="T19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>7</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>8</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="L20">
+        <v>5</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>60</v>
+      </c>
+      <c r="R20">
+        <v>5</v>
+      </c>
+      <c r="S20">
+        <v>7</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="2">
+        <v>9</v>
+      </c>
+      <c r="B21" s="3">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>75</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>43</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>13</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <v>15</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>3</v>
+      </c>
+      <c r="Q21">
+        <v>2</v>
+      </c>
+      <c r="R21">
+        <v>17</v>
+      </c>
+      <c r="S21">
+        <v>9</v>
+      </c>
+      <c r="T21">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>5</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>19</v>
+      </c>
+      <c r="T22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>582</v>
+      </c>
+      <c r="E26">
+        <v>371</v>
+      </c>
+      <c r="F26">
+        <v>421</v>
+      </c>
+      <c r="G26">
+        <v>1391</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>1525</v>
+      </c>
+      <c r="J26">
+        <v>953</v>
+      </c>
+      <c r="K26">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>418</v>
+      </c>
+      <c r="E30">
+        <v>1137</v>
+      </c>
+      <c r="F30">
+        <v>562</v>
+      </c>
+      <c r="G30">
+        <v>907</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>467</v>
+      </c>
+      <c r="J30">
+        <v>647</v>
+      </c>
+      <c r="K30">
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>